<commit_message>
Increased nuke cost and time
</commit_message>
<xml_diff>
--- a/working_dir/unitStats_Alt.xlsx
+++ b/working_dir/unitStats_Alt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\The Volt\script\RoN\RoN_UnitRules\working_dir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D154E8-CC57-4E79-8BD2-9DC81997576F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C364C0D-E3DC-49B1-98F4-300D9C3A8751}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{90FBBCC5-BA71-43FF-B8CF-06AA077B2D23}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{90FBBCC5-BA71-43FF-B8CF-06AA077B2D23}"/>
   </bookViews>
   <sheets>
     <sheet name="Upd" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="90">
   <si>
     <t>188</t>
   </si>
@@ -295,6 +295,18 @@
   </si>
   <si>
     <t>75k/90o</t>
+  </si>
+  <si>
+    <t>COST_old</t>
+  </si>
+  <si>
+    <t>10000o/10000k</t>
+  </si>
+  <si>
+    <t>50000k/60000o</t>
+  </si>
+  <si>
+    <t>75000k/90000o</t>
   </si>
 </sst>
 </file>
@@ -355,20 +367,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -380,7 +393,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -389,7 +402,7 @@
       <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -418,12 +431,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0DACEC49-E2BE-4BCF-A4FA-80AA1E89E63B}" name="Table5" displayName="Table5" ref="A1:C48" totalsRowShown="0" headerRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0DACEC49-E2BE-4BCF-A4FA-80AA1E89E63B}" name="Table5" displayName="Table5" ref="A1:C48" totalsRowShown="0" headerRowDxfId="8">
   <autoFilter ref="A1:C48" xr:uid="{56306967-8AF9-4782-A0E7-973B8E28EF62}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{64382AE9-8F04-4CA4-AC39-CABA8E967B62}" name="NAME"/>
-    <tableColumn id="2" xr3:uid="{58CC1AC5-3227-49D9-9B61-87A24867D282}" name="COST"/>
-    <tableColumn id="4" xr3:uid="{43AEB532-72FF-4785-8238-91574211164B}" name="JOB_TIME" dataDxfId="6">
+    <tableColumn id="2" xr3:uid="{58CC1AC5-3227-49D9-9B61-87A24867D282}" name="COST" dataDxfId="0">
+      <calculatedColumnFormula>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{43AEB532-72FF-4785-8238-91574211164B}" name="JOB_TIME" dataDxfId="7">
       <calculatedColumnFormula>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -432,14 +447,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{20883656-55E8-45AB-8417-BCFC28E0A0D7}" name="Table53" displayName="Table53" ref="A1:H48" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:H48" xr:uid="{56306967-8AF9-4782-A0E7-973B8E28EF62}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{20883656-55E8-45AB-8417-BCFC28E0A0D7}" name="Table53" displayName="Table53" ref="A1:I48" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A1:I48" xr:uid="{56306967-8AF9-4782-A0E7-973B8E28EF62}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{EE258F47-0C21-4BE1-9EEB-A4339E037A20}" name="NAME"/>
-    <tableColumn id="2" xr3:uid="{A761E776-832B-4961-99B0-4056D5482DD3}" name="COST"/>
+    <tableColumn id="2" xr3:uid="{A761E776-832B-4961-99B0-4056D5482DD3}" name="COST_old"/>
+    <tableColumn id="9" xr3:uid="{05E26117-DC4C-4D61-9849-C8B8F97B5E02}" name="COST"/>
     <tableColumn id="3" xr3:uid="{761EC746-FAA7-4255-BE15-B7ADF4D6B316}" name="JOB_TIME_old"/>
     <tableColumn id="5" xr3:uid="{E1929CB6-2B84-42DA-A25E-64F15064068C}" name="Rate"/>
-    <tableColumn id="4" xr3:uid="{823D3F51-9FF9-4D7B-8329-9BE1A6B9DFFD}" name="JOB_TIME" dataDxfId="1">
+    <tableColumn id="4" xr3:uid="{823D3F51-9FF9-4D7B-8329-9BE1A6B9DFFD}" name="JOB_TIME" dataDxfId="5">
       <calculatedColumnFormula>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{8EB13955-07D7-4C75-A53D-14C62104AD6D}" name="Old Time" dataDxfId="4" dataCellStyle="Comma">
@@ -775,15 +791,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{883ADAE2-84CE-46FC-8E4C-E364ED760019}">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A47" sqref="A47"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -802,8 +818,9 @@
       <c r="A2" t="s">
         <v>68</v>
       </c>
-      <c r="B2" t="s">
-        <v>67</v>
+      <c r="B2" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>4t</v>
       </c>
       <c r="C2">
         <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
@@ -814,8 +831,9 @@
       <c r="A3" t="s">
         <v>66</v>
       </c>
-      <c r="B3" t="s">
-        <v>65</v>
+      <c r="B3" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>3t/2g</v>
       </c>
       <c r="C3">
         <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
@@ -826,8 +844,9 @@
       <c r="A4" t="s">
         <v>64</v>
       </c>
-      <c r="B4" t="s">
-        <v>63</v>
+      <c r="B4" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>3g/3g</v>
       </c>
       <c r="C4">
         <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
@@ -838,8 +857,9 @@
       <c r="A5" t="s">
         <v>62</v>
       </c>
-      <c r="B5" t="s">
-        <v>61</v>
+      <c r="B5" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>3t/3g</v>
       </c>
       <c r="C5">
         <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
@@ -850,8 +870,9 @@
       <c r="A6" t="s">
         <v>60</v>
       </c>
-      <c r="B6" t="s">
-        <v>10</v>
+      <c r="B6" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>3t/3f</v>
       </c>
       <c r="C6">
         <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
@@ -862,8 +883,9 @@
       <c r="A7" t="s">
         <v>59</v>
       </c>
-      <c r="B7" t="s">
-        <v>58</v>
+      <c r="B7" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>3m/3o</v>
       </c>
       <c r="C7">
         <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
@@ -874,8 +896,9 @@
       <c r="A8" t="s">
         <v>56</v>
       </c>
-      <c r="B8" t="s">
-        <v>10</v>
+      <c r="B8" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>3t/3f</v>
       </c>
       <c r="C8">
         <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
@@ -886,8 +909,9 @@
       <c r="A9" t="s">
         <v>55</v>
       </c>
-      <c r="B9" t="s">
-        <v>10</v>
+      <c r="B9" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>3t/3f</v>
       </c>
       <c r="C9">
         <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
@@ -898,8 +922,9 @@
       <c r="A10" t="s">
         <v>54</v>
       </c>
-      <c r="B10" t="s">
-        <v>10</v>
+      <c r="B10" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>3t/3f</v>
       </c>
       <c r="C10">
         <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
@@ -910,8 +935,9 @@
       <c r="A11" t="s">
         <v>53</v>
       </c>
-      <c r="B11" t="s">
-        <v>10</v>
+      <c r="B11" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>3t/3f</v>
       </c>
       <c r="C11">
         <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
@@ -922,8 +948,9 @@
       <c r="A12" t="s">
         <v>52</v>
       </c>
-      <c r="B12" t="s">
-        <v>10</v>
+      <c r="B12" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>3t/3f</v>
       </c>
       <c r="C12">
         <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
@@ -934,8 +961,9 @@
       <c r="A13" t="s">
         <v>51</v>
       </c>
-      <c r="B13" t="s">
-        <v>48</v>
+      <c r="B13" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>7m/7o</v>
       </c>
       <c r="C13">
         <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
@@ -946,8 +974,9 @@
       <c r="A14" t="s">
         <v>50</v>
       </c>
-      <c r="B14" t="s">
-        <v>48</v>
+      <c r="B14" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>7m/7o</v>
       </c>
       <c r="C14">
         <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
@@ -958,8 +987,9 @@
       <c r="A15" t="s">
         <v>49</v>
       </c>
-      <c r="B15" t="s">
-        <v>48</v>
+      <c r="B15" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>7m/7o</v>
       </c>
       <c r="C15">
         <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
@@ -970,8 +1000,9 @@
       <c r="A16" t="s">
         <v>47</v>
       </c>
-      <c r="B16" t="s">
-        <v>10</v>
+      <c r="B16" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>3t/3f</v>
       </c>
       <c r="C16">
         <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
@@ -982,8 +1013,9 @@
       <c r="A17" t="s">
         <v>46</v>
       </c>
-      <c r="B17" t="s">
-        <v>10</v>
+      <c r="B17" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>3t/3f</v>
       </c>
       <c r="C17">
         <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
@@ -994,8 +1026,9 @@
       <c r="A18" t="s">
         <v>45</v>
       </c>
-      <c r="B18" t="s">
-        <v>10</v>
+      <c r="B18" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>3t/3f</v>
       </c>
       <c r="C18">
         <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
@@ -1006,8 +1039,9 @@
       <c r="A19" t="s">
         <v>44</v>
       </c>
-      <c r="B19" t="s">
-        <v>42</v>
+      <c r="B19" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>2t/4g</v>
       </c>
       <c r="C19">
         <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
@@ -1018,8 +1052,9 @@
       <c r="A20" t="s">
         <v>43</v>
       </c>
-      <c r="B20" t="s">
-        <v>42</v>
+      <c r="B20" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>2t/4g</v>
       </c>
       <c r="C20">
         <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
@@ -1030,8 +1065,9 @@
       <c r="A21" t="s">
         <v>41</v>
       </c>
-      <c r="B21" t="s">
-        <v>39</v>
+      <c r="B21" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>3t/6g</v>
       </c>
       <c r="C21">
         <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
@@ -1042,8 +1078,9 @@
       <c r="A22" t="s">
         <v>40</v>
       </c>
-      <c r="B22" t="s">
-        <v>39</v>
+      <c r="B22" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>3t/6g</v>
       </c>
       <c r="C22">
         <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
@@ -1054,8 +1091,9 @@
       <c r="A23" t="s">
         <v>38</v>
       </c>
-      <c r="B23" t="s">
-        <v>8</v>
+      <c r="B23" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>6o/8g</v>
       </c>
       <c r="C23">
         <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
@@ -1066,8 +1104,9 @@
       <c r="A24" t="s">
         <v>37</v>
       </c>
-      <c r="B24" t="s">
-        <v>8</v>
+      <c r="B24" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>6o/8g</v>
       </c>
       <c r="C24">
         <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
@@ -1078,8 +1117,9 @@
       <c r="A25" t="s">
         <v>36</v>
       </c>
-      <c r="B25" t="s">
-        <v>33</v>
+      <c r="B25" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>4t/4m</v>
       </c>
       <c r="C25">
         <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
@@ -1090,8 +1130,9 @@
       <c r="A26" t="s">
         <v>35</v>
       </c>
-      <c r="B26" t="s">
-        <v>33</v>
+      <c r="B26" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>4t/4m</v>
       </c>
       <c r="C26">
         <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
@@ -1102,8 +1143,9 @@
       <c r="A27" t="s">
         <v>34</v>
       </c>
-      <c r="B27" t="s">
-        <v>33</v>
+      <c r="B27" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>4t/4m</v>
       </c>
       <c r="C27">
         <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
@@ -1114,8 +1156,9 @@
       <c r="A28" t="s">
         <v>32</v>
       </c>
-      <c r="B28" t="s">
-        <v>30</v>
+      <c r="B28" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>6t/6m</v>
       </c>
       <c r="C28">
         <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
@@ -1126,8 +1169,9 @@
       <c r="A29" t="s">
         <v>31</v>
       </c>
-      <c r="B29" t="s">
-        <v>30</v>
+      <c r="B29" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>6t/6m</v>
       </c>
       <c r="C29">
         <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
@@ -1138,8 +1182,9 @@
       <c r="A30" t="s">
         <v>29</v>
       </c>
-      <c r="B30" t="s">
-        <v>5</v>
+      <c r="B30" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>8t/8m</v>
       </c>
       <c r="C30">
         <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
@@ -1150,8 +1195,9 @@
       <c r="A31" t="s">
         <v>28</v>
       </c>
-      <c r="B31" t="s">
-        <v>5</v>
+      <c r="B31" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>8t/8m</v>
       </c>
       <c r="C31">
         <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
@@ -1162,8 +1208,9 @@
       <c r="A32" t="s">
         <v>27</v>
       </c>
-      <c r="B32" t="s">
-        <v>5</v>
+      <c r="B32" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>8t/8m</v>
       </c>
       <c r="C32">
         <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
@@ -1174,8 +1221,9 @@
       <c r="A33" t="s">
         <v>26</v>
       </c>
-      <c r="B33" t="s">
-        <v>23</v>
+      <c r="B33" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>14m/9o</v>
       </c>
       <c r="C33">
         <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
@@ -1186,8 +1234,9 @@
       <c r="A34" t="s">
         <v>25</v>
       </c>
-      <c r="B34" t="s">
-        <v>23</v>
+      <c r="B34" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>14m/9o</v>
       </c>
       <c r="C34">
         <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
@@ -1198,8 +1247,9 @@
       <c r="A35" t="s">
         <v>24</v>
       </c>
-      <c r="B35" t="s">
-        <v>23</v>
+      <c r="B35" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>14m/9o</v>
       </c>
       <c r="C35">
         <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
@@ -1210,8 +1260,9 @@
       <c r="A36" t="s">
         <v>22</v>
       </c>
-      <c r="B36" t="s">
-        <v>21</v>
+      <c r="B36" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>65g/65o</v>
       </c>
       <c r="C36">
         <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
@@ -1222,8 +1273,9 @@
       <c r="A37" t="s">
         <v>19</v>
       </c>
-      <c r="B37" t="s">
-        <v>18</v>
+      <c r="B37" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>7t/7m</v>
       </c>
       <c r="C37">
         <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
@@ -1234,8 +1286,9 @@
       <c r="A38" t="s">
         <v>17</v>
       </c>
-      <c r="B38" t="s">
-        <v>16</v>
+      <c r="B38" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>5t/3o</v>
       </c>
       <c r="C38">
         <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
@@ -1246,8 +1299,9 @@
       <c r="A39" t="s">
         <v>14</v>
       </c>
-      <c r="B39" t="s">
-        <v>13</v>
+      <c r="B39" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>8t/6m</v>
       </c>
       <c r="C39">
         <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
@@ -1258,8 +1312,9 @@
       <c r="A40" t="s">
         <v>11</v>
       </c>
-      <c r="B40" t="s">
-        <v>10</v>
+      <c r="B40" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>3t/3f</v>
       </c>
       <c r="C40">
         <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
@@ -1270,8 +1325,9 @@
       <c r="A41" t="s">
         <v>9</v>
       </c>
-      <c r="B41" t="s">
-        <v>8</v>
+      <c r="B41" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>6o/8g</v>
       </c>
       <c r="C41">
         <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
@@ -1282,8 +1338,9 @@
       <c r="A42" t="s">
         <v>6</v>
       </c>
-      <c r="B42" t="s">
-        <v>5</v>
+      <c r="B42" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>8t/8m</v>
       </c>
       <c r="C42">
         <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
@@ -1294,8 +1351,9 @@
       <c r="A43" t="s">
         <v>3</v>
       </c>
-      <c r="B43" t="s">
-        <v>1</v>
+      <c r="B43" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>3f</v>
       </c>
       <c r="C43">
         <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
@@ -1306,8 +1364,9 @@
       <c r="A44" t="s">
         <v>2</v>
       </c>
-      <c r="B44" t="s">
-        <v>1</v>
+      <c r="B44" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>3f</v>
       </c>
       <c r="C44">
         <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
@@ -1318,48 +1377,52 @@
       <c r="A45" t="s">
         <v>76</v>
       </c>
-      <c r="B45" t="s">
-        <v>77</v>
-      </c>
-      <c r="C45" s="5">
-        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
-        <v>17000</v>
+      <c r="B45" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>10000o/10000k</v>
+      </c>
+      <c r="C45">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
+        <v>85000</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>79</v>
       </c>
-      <c r="B46" t="s">
-        <v>80</v>
-      </c>
-      <c r="C46" s="5">
-        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
-        <v>60000</v>
+      <c r="B46" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>50000k/60000o</v>
+      </c>
+      <c r="C46">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
+        <v>300000</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>83</v>
       </c>
-      <c r="B47" t="s">
-        <v>77</v>
-      </c>
-      <c r="C47" s="5">
-        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
-        <v>17000</v>
+      <c r="B47" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>10000o/10000k</v>
+      </c>
+      <c r="C47">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
+        <v>85000</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>84</v>
       </c>
-      <c r="B48" t="s">
-        <v>85</v>
-      </c>
-      <c r="C48" s="5">
-        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
-        <v>60000</v>
+      <c r="B48" t="str">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[COST])</f>
+        <v>75000k/90000o</v>
+      </c>
+      <c r="C48">
+        <f>_xlfn.XLOOKUP(Table5[[#This Row],[NAME]],Table53[NAME],Table53[JOB_TIME],0)</f>
+        <v>300000</v>
       </c>
     </row>
   </sheetData>
@@ -1372,52 +1435,56 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07D39A8D-D416-44B4-9959-0FDE0CC4DD67}">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D46" sqref="D46"/>
+      <selection pane="bottomLeft" activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -1425,29 +1492,32 @@
         <v>67</v>
       </c>
       <c r="C2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" t="s">
         <v>57</v>
       </c>
-      <c r="D2">
-        <v>75</v>
-      </c>
       <c r="E2">
+        <v>75</v>
+      </c>
+      <c r="F2">
         <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
         <v>7050</v>
       </c>
-      <c r="F2" s="2" t="str">
+      <c r="G2" s="2" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>7.5 sec</v>
       </c>
-      <c r="G2" s="2" t="str">
+      <c r="H2" s="2" t="str">
         <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>564.0 sec</v>
       </c>
-      <c r="H2" s="2" t="str">
+      <c r="I2" s="2" t="str">
         <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
         <v>9.4 min</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>66</v>
       </c>
@@ -1455,30 +1525,33 @@
         <v>65</v>
       </c>
       <c r="C3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" t="s">
         <v>57</v>
       </c>
-      <c r="D3">
-        <f>D2</f>
-        <v>75</v>
-      </c>
       <c r="E3">
+        <f>E2</f>
+        <v>75</v>
+      </c>
+      <c r="F3">
         <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
         <v>7050</v>
       </c>
-      <c r="F3" s="2" t="str">
+      <c r="G3" s="2" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>7.5 sec</v>
       </c>
-      <c r="G3" s="2" t="str">
+      <c r="H3" s="2" t="str">
         <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>564.0 sec</v>
       </c>
-      <c r="H3" s="2" t="str">
+      <c r="I3" s="2" t="str">
         <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
         <v>9.4 min</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -1486,30 +1559,33 @@
         <v>63</v>
       </c>
       <c r="C4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" t="s">
         <v>57</v>
       </c>
-      <c r="D4">
-        <f t="shared" ref="D4:D48" si="0">D3</f>
-        <v>75</v>
-      </c>
       <c r="E4">
+        <f t="shared" ref="E4:E48" si="0">E3</f>
+        <v>75</v>
+      </c>
+      <c r="F4">
         <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
         <v>7050</v>
       </c>
-      <c r="F4" s="2" t="str">
+      <c r="G4" s="2" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>7.5 sec</v>
       </c>
-      <c r="G4" s="2" t="str">
+      <c r="H4" s="2" t="str">
         <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>564.0 sec</v>
       </c>
-      <c r="H4" s="2" t="str">
+      <c r="I4" s="2" t="str">
         <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
         <v>9.4 min</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>62</v>
       </c>
@@ -1517,30 +1593,33 @@
         <v>61</v>
       </c>
       <c r="C5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" t="s">
         <v>57</v>
       </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
       <c r="E5">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F5">
         <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
         <v>7050</v>
       </c>
-      <c r="F5" s="2" t="str">
+      <c r="G5" s="2" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>7.5 sec</v>
       </c>
-      <c r="G5" s="2" t="str">
+      <c r="H5" s="2" t="str">
         <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>564.0 sec</v>
       </c>
-      <c r="H5" s="2" t="str">
+      <c r="I5" s="2" t="str">
         <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
         <v>9.4 min</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>60</v>
       </c>
@@ -1548,30 +1627,33 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
         <v>57</v>
       </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
       <c r="E6">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F6">
         <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
         <v>7050</v>
       </c>
-      <c r="F6" s="2" t="str">
+      <c r="G6" s="2" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>7.5 sec</v>
       </c>
-      <c r="G6" s="2" t="str">
+      <c r="H6" s="2" t="str">
         <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>564.0 sec</v>
       </c>
-      <c r="H6" s="2" t="str">
+      <c r="I6" s="2" t="str">
         <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
         <v>9.4 min</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>59</v>
       </c>
@@ -1579,30 +1661,33 @@
         <v>58</v>
       </c>
       <c r="C7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" t="s">
         <v>57</v>
       </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
       <c r="E7">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F7">
         <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
         <v>7050</v>
       </c>
-      <c r="F7" s="2" t="str">
+      <c r="G7" s="2" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>7.5 sec</v>
       </c>
-      <c r="G7" s="2" t="str">
+      <c r="H7" s="2" t="str">
         <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>564.0 sec</v>
       </c>
-      <c r="H7" s="2" t="str">
+      <c r="I7" s="2" t="str">
         <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
         <v>9.4 min</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -1610,30 +1695,33 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
         <v>7</v>
       </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
       <c r="E8">
-        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
-        <v>11250</v>
-      </c>
-      <c r="F8" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F8">
+        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
+        <v>11250</v>
+      </c>
+      <c r="G8" s="2" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>12.0 sec</v>
       </c>
-      <c r="G8" s="2" t="str">
+      <c r="H8" s="2" t="str">
         <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>900.0 sec</v>
       </c>
-      <c r="H8" s="2" t="str">
+      <c r="I8" s="2" t="str">
         <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
         <v>15.0 min</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -1641,30 +1729,33 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
         <v>7</v>
       </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
       <c r="E9">
-        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
-        <v>11250</v>
-      </c>
-      <c r="F9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F9">
+        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
+        <v>11250</v>
+      </c>
+      <c r="G9" s="2" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>12.0 sec</v>
       </c>
-      <c r="G9" s="2" t="str">
+      <c r="H9" s="2" t="str">
         <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>900.0 sec</v>
       </c>
-      <c r="H9" s="2" t="str">
+      <c r="I9" s="2" t="str">
         <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
         <v>15.0 min</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>54</v>
       </c>
@@ -1672,30 +1763,33 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
         <v>7</v>
       </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
       <c r="E10">
-        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
-        <v>11250</v>
-      </c>
-      <c r="F10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F10">
+        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
+        <v>11250</v>
+      </c>
+      <c r="G10" s="2" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>12.0 sec</v>
       </c>
-      <c r="G10" s="2" t="str">
+      <c r="H10" s="2" t="str">
         <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>900.0 sec</v>
       </c>
-      <c r="H10" s="2" t="str">
+      <c r="I10" s="2" t="str">
         <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
         <v>15.0 min</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -1703,30 +1797,33 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
         <v>7</v>
       </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
       <c r="E11">
-        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
-        <v>11250</v>
-      </c>
-      <c r="F11" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F11">
+        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
+        <v>11250</v>
+      </c>
+      <c r="G11" s="2" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>12.0 sec</v>
       </c>
-      <c r="G11" s="2" t="str">
+      <c r="H11" s="2" t="str">
         <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>900.0 sec</v>
       </c>
-      <c r="H11" s="2" t="str">
+      <c r="I11" s="2" t="str">
         <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
         <v>15.0 min</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -1734,30 +1831,33 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
         <v>7</v>
       </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
       <c r="E12">
-        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
-        <v>11250</v>
-      </c>
-      <c r="F12" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F12">
+        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
+        <v>11250</v>
+      </c>
+      <c r="G12" s="2" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>12.0 sec</v>
       </c>
-      <c r="G12" s="2" t="str">
+      <c r="H12" s="2" t="str">
         <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>900.0 sec</v>
       </c>
-      <c r="H12" s="2" t="str">
+      <c r="I12" s="2" t="str">
         <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
         <v>15.0 min</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -1765,30 +1865,33 @@
         <v>48</v>
       </c>
       <c r="C13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" t="s">
         <v>7</v>
       </c>
-      <c r="D13">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
       <c r="E13">
-        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
-        <v>11250</v>
-      </c>
-      <c r="F13" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F13">
+        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
+        <v>11250</v>
+      </c>
+      <c r="G13" s="2" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>12.0 sec</v>
       </c>
-      <c r="G13" s="2" t="str">
+      <c r="H13" s="2" t="str">
         <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>900.0 sec</v>
       </c>
-      <c r="H13" s="2" t="str">
+      <c r="I13" s="2" t="str">
         <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
         <v>15.0 min</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -1796,30 +1899,33 @@
         <v>48</v>
       </c>
       <c r="C14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" t="s">
         <v>7</v>
       </c>
-      <c r="D14">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
       <c r="E14">
-        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
-        <v>11250</v>
-      </c>
-      <c r="F14" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F14">
+        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
+        <v>11250</v>
+      </c>
+      <c r="G14" s="2" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>12.0 sec</v>
       </c>
-      <c r="G14" s="2" t="str">
+      <c r="H14" s="2" t="str">
         <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>900.0 sec</v>
       </c>
-      <c r="H14" s="2" t="str">
+      <c r="I14" s="2" t="str">
         <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
         <v>15.0 min</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>49</v>
       </c>
@@ -1827,30 +1933,33 @@
         <v>48</v>
       </c>
       <c r="C15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" t="s">
         <v>7</v>
       </c>
-      <c r="D15">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
       <c r="E15">
-        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
-        <v>11250</v>
-      </c>
-      <c r="F15" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F15">
+        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
+        <v>11250</v>
+      </c>
+      <c r="G15" s="2" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>12.0 sec</v>
       </c>
-      <c r="G15" s="2" t="str">
+      <c r="H15" s="2" t="str">
         <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>900.0 sec</v>
       </c>
-      <c r="H15" s="2" t="str">
+      <c r="I15" s="2" t="str">
         <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
         <v>15.0 min</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -1858,30 +1967,33 @@
         <v>10</v>
       </c>
       <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
         <v>7</v>
       </c>
-      <c r="D16">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
       <c r="E16">
-        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
-        <v>11250</v>
-      </c>
-      <c r="F16" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F16">
+        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
+        <v>11250</v>
+      </c>
+      <c r="G16" s="2" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>12.0 sec</v>
       </c>
-      <c r="G16" s="2" t="str">
+      <c r="H16" s="2" t="str">
         <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>900.0 sec</v>
       </c>
-      <c r="H16" s="2" t="str">
+      <c r="I16" s="2" t="str">
         <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
         <v>15.0 min</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -1889,30 +2001,33 @@
         <v>10</v>
       </c>
       <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" t="s">
         <v>7</v>
       </c>
-      <c r="D17">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
       <c r="E17">
-        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
-        <v>11250</v>
-      </c>
-      <c r="F17" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F17">
+        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
+        <v>11250</v>
+      </c>
+      <c r="G17" s="2" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>12.0 sec</v>
       </c>
-      <c r="G17" s="2" t="str">
+      <c r="H17" s="2" t="str">
         <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>900.0 sec</v>
       </c>
-      <c r="H17" s="2" t="str">
+      <c r="I17" s="2" t="str">
         <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
         <v>15.0 min</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -1920,30 +2035,33 @@
         <v>10</v>
       </c>
       <c r="C18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" t="s">
         <v>7</v>
       </c>
-      <c r="D18">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
       <c r="E18">
-        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
-        <v>11250</v>
-      </c>
-      <c r="F18" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F18">
+        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
+        <v>11250</v>
+      </c>
+      <c r="G18" s="2" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>12.0 sec</v>
       </c>
-      <c r="G18" s="2" t="str">
+      <c r="H18" s="2" t="str">
         <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>900.0 sec</v>
       </c>
-      <c r="H18" s="2" t="str">
+      <c r="I18" s="2" t="str">
         <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
         <v>15.0 min</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -1951,30 +2069,33 @@
         <v>42</v>
       </c>
       <c r="C19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" t="s">
         <v>7</v>
       </c>
-      <c r="D19">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
       <c r="E19">
-        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
-        <v>11250</v>
-      </c>
-      <c r="F19" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F19">
+        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
+        <v>11250</v>
+      </c>
+      <c r="G19" s="2" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>12.0 sec</v>
       </c>
-      <c r="G19" s="2" t="str">
+      <c r="H19" s="2" t="str">
         <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>900.0 sec</v>
       </c>
-      <c r="H19" s="2" t="str">
+      <c r="I19" s="2" t="str">
         <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
         <v>15.0 min</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -1982,30 +2103,33 @@
         <v>42</v>
       </c>
       <c r="C20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" t="s">
         <v>7</v>
       </c>
-      <c r="D20">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
       <c r="E20">
-        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
-        <v>11250</v>
-      </c>
-      <c r="F20" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F20">
+        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
+        <v>11250</v>
+      </c>
+      <c r="G20" s="2" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>12.0 sec</v>
       </c>
-      <c r="G20" s="2" t="str">
+      <c r="H20" s="2" t="str">
         <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>900.0 sec</v>
       </c>
-      <c r="H20" s="2" t="str">
+      <c r="I20" s="2" t="str">
         <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
         <v>15.0 min</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -2013,30 +2137,33 @@
         <v>39</v>
       </c>
       <c r="C21" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" t="s">
         <v>7</v>
       </c>
-      <c r="D21">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
       <c r="E21">
-        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
-        <v>11250</v>
-      </c>
-      <c r="F21" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F21">
+        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
+        <v>11250</v>
+      </c>
+      <c r="G21" s="2" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>12.0 sec</v>
       </c>
-      <c r="G21" s="2" t="str">
+      <c r="H21" s="2" t="str">
         <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>900.0 sec</v>
       </c>
-      <c r="H21" s="2" t="str">
+      <c r="I21" s="2" t="str">
         <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
         <v>15.0 min</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -2044,30 +2171,33 @@
         <v>39</v>
       </c>
       <c r="C22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" t="s">
         <v>7</v>
       </c>
-      <c r="D22">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
       <c r="E22">
-        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
-        <v>11250</v>
-      </c>
-      <c r="F22" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F22">
+        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
+        <v>11250</v>
+      </c>
+      <c r="G22" s="2" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>12.0 sec</v>
       </c>
-      <c r="G22" s="2" t="str">
+      <c r="H22" s="2" t="str">
         <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>900.0 sec</v>
       </c>
-      <c r="H22" s="2" t="str">
+      <c r="I22" s="2" t="str">
         <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
         <v>15.0 min</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -2075,30 +2205,33 @@
         <v>8</v>
       </c>
       <c r="C23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" t="s">
         <v>7</v>
       </c>
-      <c r="D23">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
       <c r="E23">
-        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
-        <v>11250</v>
-      </c>
-      <c r="F23" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F23">
+        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
+        <v>11250</v>
+      </c>
+      <c r="G23" s="2" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>12.0 sec</v>
       </c>
-      <c r="G23" s="2" t="str">
+      <c r="H23" s="2" t="str">
         <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>900.0 sec</v>
       </c>
-      <c r="H23" s="2" t="str">
+      <c r="I23" s="2" t="str">
         <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
         <v>15.0 min</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -2106,30 +2239,33 @@
         <v>8</v>
       </c>
       <c r="C24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" t="s">
         <v>7</v>
       </c>
-      <c r="D24">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
       <c r="E24">
-        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
-        <v>11250</v>
-      </c>
-      <c r="F24" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F24">
+        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
+        <v>11250</v>
+      </c>
+      <c r="G24" s="2" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>12.0 sec</v>
       </c>
-      <c r="G24" s="2" t="str">
+      <c r="H24" s="2" t="str">
         <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>900.0 sec</v>
       </c>
-      <c r="H24" s="2" t="str">
+      <c r="I24" s="2" t="str">
         <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
         <v>15.0 min</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -2137,30 +2273,33 @@
         <v>33</v>
       </c>
       <c r="C25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" t="s">
         <v>12</v>
       </c>
-      <c r="D25">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
       <c r="E25">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F25">
         <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
         <v>16875</v>
       </c>
-      <c r="F25" s="2" t="str">
+      <c r="G25" s="2" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>18.0 sec</v>
       </c>
-      <c r="G25" s="2" t="str">
+      <c r="H25" s="2" t="str">
         <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>1,350.0 sec</v>
       </c>
-      <c r="H25" s="2" t="str">
+      <c r="I25" s="2" t="str">
         <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
         <v>22.5 min</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -2168,30 +2307,33 @@
         <v>33</v>
       </c>
       <c r="C26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" t="s">
         <v>12</v>
       </c>
-      <c r="D26">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
       <c r="E26">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F26">
         <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
         <v>16875</v>
       </c>
-      <c r="F26" s="2" t="str">
+      <c r="G26" s="2" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>18.0 sec</v>
       </c>
-      <c r="G26" s="2" t="str">
+      <c r="H26" s="2" t="str">
         <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>1,350.0 sec</v>
       </c>
-      <c r="H26" s="2" t="str">
+      <c r="I26" s="2" t="str">
         <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
         <v>22.5 min</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>34</v>
       </c>
@@ -2199,30 +2341,33 @@
         <v>33</v>
       </c>
       <c r="C27" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D27" s="3">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
       <c r="E27" s="3">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F27" s="3">
         <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
         <v>16875</v>
       </c>
-      <c r="F27" s="4" t="str">
+      <c r="G27" s="4" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>18.0 sec</v>
       </c>
-      <c r="G27" s="4" t="str">
+      <c r="H27" s="4" t="str">
         <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>1,350.0 sec</v>
       </c>
-      <c r="H27" s="4" t="str">
+      <c r="I27" s="4" t="str">
         <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
         <v>22.5 min</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>32</v>
       </c>
@@ -2230,30 +2375,33 @@
         <v>30</v>
       </c>
       <c r="C28" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D28" s="3">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
       <c r="E28" s="3">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F28" s="3">
         <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
         <v>16875</v>
       </c>
-      <c r="F28" s="4" t="str">
+      <c r="G28" s="4" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>18.0 sec</v>
       </c>
-      <c r="G28" s="4" t="str">
+      <c r="H28" s="4" t="str">
         <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>1,350.0 sec</v>
       </c>
-      <c r="H28" s="4" t="str">
+      <c r="I28" s="4" t="str">
         <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
         <v>22.5 min</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>31</v>
       </c>
@@ -2261,30 +2409,33 @@
         <v>30</v>
       </c>
       <c r="C29" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D29" s="3">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
       <c r="E29" s="3">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F29" s="3">
         <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
         <v>16875</v>
       </c>
-      <c r="F29" s="4" t="str">
+      <c r="G29" s="4" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>18.0 sec</v>
       </c>
-      <c r="G29" s="4" t="str">
+      <c r="H29" s="4" t="str">
         <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>1,350.0 sec</v>
       </c>
-      <c r="H29" s="4" t="str">
+      <c r="I29" s="4" t="str">
         <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
         <v>22.5 min</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>29</v>
       </c>
@@ -2292,30 +2443,33 @@
         <v>5</v>
       </c>
       <c r="C30" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D30" s="3">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
       <c r="E30" s="3">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F30" s="3">
         <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
         <v>22500</v>
       </c>
-      <c r="F30" s="4" t="str">
+      <c r="G30" s="4" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>24.0 sec</v>
       </c>
-      <c r="G30" s="4" t="str">
+      <c r="H30" s="4" t="str">
         <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>1,800.0 sec</v>
       </c>
-      <c r="H30" s="4" t="str">
+      <c r="I30" s="4" t="str">
         <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
         <v>30.0 min</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>28</v>
       </c>
@@ -2323,30 +2477,33 @@
         <v>5</v>
       </c>
       <c r="C31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D31" s="3">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
       <c r="E31" s="3">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F31" s="3">
         <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
         <v>22500</v>
       </c>
-      <c r="F31" s="4" t="str">
+      <c r="G31" s="4" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>24.0 sec</v>
       </c>
-      <c r="G31" s="4" t="str">
+      <c r="H31" s="4" t="str">
         <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>1,800.0 sec</v>
       </c>
-      <c r="H31" s="4" t="str">
+      <c r="I31" s="4" t="str">
         <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
         <v>30.0 min</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>27</v>
       </c>
@@ -2354,30 +2511,33 @@
         <v>5</v>
       </c>
       <c r="C32" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D32" s="3">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
       <c r="E32" s="3">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F32" s="3">
         <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
         <v>22500</v>
       </c>
-      <c r="F32" s="4" t="str">
+      <c r="G32" s="4" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>24.0 sec</v>
       </c>
-      <c r="G32" s="4" t="str">
+      <c r="H32" s="4" t="str">
         <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>1,800.0 sec</v>
       </c>
-      <c r="H32" s="4" t="str">
+      <c r="I32" s="4" t="str">
         <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
         <v>30.0 min</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>26</v>
       </c>
@@ -2385,30 +2545,33 @@
         <v>23</v>
       </c>
       <c r="C33" t="s">
+        <v>23</v>
+      </c>
+      <c r="D33" t="s">
         <v>4</v>
       </c>
-      <c r="D33">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
       <c r="E33">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F33">
         <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
         <v>22500</v>
       </c>
-      <c r="F33" s="2" t="str">
+      <c r="G33" s="2" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>24.0 sec</v>
       </c>
-      <c r="G33" s="2" t="str">
+      <c r="H33" s="2" t="str">
         <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>1,800.0 sec</v>
       </c>
-      <c r="H33" s="2" t="str">
+      <c r="I33" s="2" t="str">
         <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
         <v>30.0 min</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>25</v>
       </c>
@@ -2416,30 +2579,33 @@
         <v>23</v>
       </c>
       <c r="C34" t="s">
+        <v>23</v>
+      </c>
+      <c r="D34" t="s">
         <v>4</v>
       </c>
-      <c r="D34">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
       <c r="E34">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F34">
         <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
         <v>22500</v>
       </c>
-      <c r="F34" s="2" t="str">
+      <c r="G34" s="2" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>24.0 sec</v>
       </c>
-      <c r="G34" s="2" t="str">
+      <c r="H34" s="2" t="str">
         <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>1,800.0 sec</v>
       </c>
-      <c r="H34" s="2" t="str">
+      <c r="I34" s="2" t="str">
         <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
         <v>30.0 min</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>24</v>
       </c>
@@ -2447,30 +2613,33 @@
         <v>23</v>
       </c>
       <c r="C35" t="s">
+        <v>23</v>
+      </c>
+      <c r="D35" t="s">
         <v>4</v>
       </c>
-      <c r="D35">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
       <c r="E35">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F35">
         <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
         <v>22500</v>
       </c>
-      <c r="F35" s="2" t="str">
+      <c r="G35" s="2" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>24.0 sec</v>
       </c>
-      <c r="G35" s="2" t="str">
+      <c r="H35" s="2" t="str">
         <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>1,800.0 sec</v>
       </c>
-      <c r="H35" s="2" t="str">
+      <c r="I35" s="2" t="str">
         <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
         <v>30.0 min</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -2478,30 +2647,33 @@
         <v>21</v>
       </c>
       <c r="C36" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36" t="s">
         <v>20</v>
       </c>
-      <c r="D36">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
       <c r="E36">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F36">
         <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
         <v>18750</v>
       </c>
-      <c r="F36" s="2" t="str">
+      <c r="G36" s="2" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>20.0 sec</v>
       </c>
-      <c r="G36" s="2" t="str">
+      <c r="H36" s="2" t="str">
         <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>1,500.0 sec</v>
       </c>
-      <c r="H36" s="2" t="str">
+      <c r="I36" s="2" t="str">
         <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
         <v>25.0 min</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>19</v>
       </c>
@@ -2509,30 +2681,33 @@
         <v>18</v>
       </c>
       <c r="C37" t="s">
+        <v>18</v>
+      </c>
+      <c r="D37" t="s">
         <v>12</v>
       </c>
-      <c r="D37">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
       <c r="E37">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F37">
         <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
         <v>16875</v>
       </c>
-      <c r="F37" s="2" t="str">
+      <c r="G37" s="2" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>18.0 sec</v>
       </c>
-      <c r="G37" s="2" t="str">
+      <c r="H37" s="2" t="str">
         <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>1,350.0 sec</v>
       </c>
-      <c r="H37" s="2" t="str">
+      <c r="I37" s="2" t="str">
         <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
         <v>22.5 min</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>17</v>
       </c>
@@ -2540,30 +2715,33 @@
         <v>16</v>
       </c>
       <c r="C38" t="s">
+        <v>16</v>
+      </c>
+      <c r="D38" t="s">
         <v>15</v>
       </c>
-      <c r="D38">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
       <c r="E38">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F38">
         <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
         <v>9000</v>
       </c>
-      <c r="F38" s="2" t="str">
+      <c r="G38" s="2" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>9.6 sec</v>
       </c>
-      <c r="G38" s="2" t="str">
+      <c r="H38" s="2" t="str">
         <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>720.0 sec</v>
       </c>
-      <c r="H38" s="2" t="str">
+      <c r="I38" s="2" t="str">
         <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
         <v>12.0 min</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -2571,30 +2749,33 @@
         <v>13</v>
       </c>
       <c r="C39" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" t="s">
         <v>12</v>
       </c>
-      <c r="D39">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
       <c r="E39">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F39">
         <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
         <v>16875</v>
       </c>
-      <c r="F39" s="2" t="str">
+      <c r="G39" s="2" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>18.0 sec</v>
       </c>
-      <c r="G39" s="2" t="str">
+      <c r="H39" s="2" t="str">
         <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>1,350.0 sec</v>
       </c>
-      <c r="H39" s="2" t="str">
+      <c r="I39" s="2" t="str">
         <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
         <v>22.5 min</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>11</v>
       </c>
@@ -2602,30 +2783,33 @@
         <v>10</v>
       </c>
       <c r="C40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" t="s">
         <v>7</v>
       </c>
-      <c r="D40">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
       <c r="E40">
-        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
-        <v>11250</v>
-      </c>
-      <c r="F40" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F40">
+        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
+        <v>11250</v>
+      </c>
+      <c r="G40" s="2" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>12.0 sec</v>
       </c>
-      <c r="G40" s="2" t="str">
+      <c r="H40" s="2" t="str">
         <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>900.0 sec</v>
       </c>
-      <c r="H40" s="2" t="str">
+      <c r="I40" s="2" t="str">
         <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
         <v>15.0 min</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>9</v>
       </c>
@@ -2633,30 +2817,33 @@
         <v>8</v>
       </c>
       <c r="C41" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" t="s">
         <v>7</v>
       </c>
-      <c r="D41">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
       <c r="E41">
-        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
-        <v>11250</v>
-      </c>
-      <c r="F41" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F41">
+        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
+        <v>11250</v>
+      </c>
+      <c r="G41" s="2" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>12.0 sec</v>
       </c>
-      <c r="G41" s="2" t="str">
+      <c r="H41" s="2" t="str">
         <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>900.0 sec</v>
       </c>
-      <c r="H41" s="2" t="str">
+      <c r="I41" s="2" t="str">
         <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
         <v>15.0 min</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>6</v>
       </c>
@@ -2664,30 +2851,33 @@
         <v>5</v>
       </c>
       <c r="C42" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" t="s">
         <v>4</v>
       </c>
-      <c r="D42">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
       <c r="E42">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F42">
         <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
         <v>22500</v>
       </c>
-      <c r="F42" s="2" t="str">
+      <c r="G42" s="2" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>24.0 sec</v>
       </c>
-      <c r="G42" s="2" t="str">
+      <c r="H42" s="2" t="str">
         <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>1,800.0 sec</v>
       </c>
-      <c r="H42" s="2" t="str">
+      <c r="I42" s="2" t="str">
         <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
         <v>30.0 min</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>3</v>
       </c>
@@ -2695,30 +2885,33 @@
         <v>1</v>
       </c>
       <c r="C43" t="s">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
         <v>0</v>
       </c>
-      <c r="D43">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
       <c r="E43">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F43">
         <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
         <v>14100</v>
       </c>
-      <c r="F43" s="2" t="str">
+      <c r="G43" s="2" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>15.0 sec</v>
       </c>
-      <c r="G43" s="2" t="str">
+      <c r="H43" s="2" t="str">
         <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>1,128.0 sec</v>
       </c>
-      <c r="H43" s="2" t="str">
+      <c r="I43" s="2" t="str">
         <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
         <v>18.8 min</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>2</v>
       </c>
@@ -2726,30 +2919,33 @@
         <v>1</v>
       </c>
       <c r="C44" t="s">
+        <v>1</v>
+      </c>
+      <c r="D44" t="s">
         <v>0</v>
       </c>
-      <c r="D44">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
       <c r="E44">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="F44">
         <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
         <v>14100</v>
       </c>
-      <c r="F44" s="2" t="str">
+      <c r="G44" s="2" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>15.0 sec</v>
       </c>
-      <c r="G44" s="2" t="str">
+      <c r="H44" s="2" t="str">
         <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>1,128.0 sec</v>
       </c>
-      <c r="H44" s="2" t="str">
+      <c r="I44" s="2" t="str">
         <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
         <v>18.8 min</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>76</v>
       </c>
@@ -2757,29 +2953,32 @@
         <v>77</v>
       </c>
       <c r="C45" t="s">
+        <v>87</v>
+      </c>
+      <c r="D45" t="s">
         <v>78</v>
       </c>
-      <c r="D45">
-        <v>100</v>
-      </c>
-      <c r="E45" s="5">
-        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
-        <v>17000</v>
-      </c>
-      <c r="F45" s="6" t="str">
+      <c r="E45">
+        <v>500</v>
+      </c>
+      <c r="F45">
+        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
+        <v>85000</v>
+      </c>
+      <c r="G45" s="2" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>13.6 sec</v>
       </c>
-      <c r="G45" s="6" t="str">
-        <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
-        <v>1,360.0 sec</v>
-      </c>
-      <c r="H45" s="6" t="str">
-        <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
-        <v>22.7 min</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H45" s="2" t="str">
+        <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
+        <v>6,800.0 sec</v>
+      </c>
+      <c r="I45" s="2" t="str">
+        <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
+        <v>113.3 min</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>79</v>
       </c>
@@ -2787,30 +2986,33 @@
         <v>80</v>
       </c>
       <c r="C46" t="s">
+        <v>88</v>
+      </c>
+      <c r="D46" t="s">
         <v>81</v>
       </c>
-      <c r="D46">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="E46" s="5">
-        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
-        <v>60000</v>
-      </c>
-      <c r="F46" s="6" t="str">
+      <c r="E46">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="F46">
+        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
+        <v>300000</v>
+      </c>
+      <c r="G46" s="2" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>48.0 sec</v>
       </c>
-      <c r="G46" s="6" t="str">
-        <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
-        <v>4,800.0 sec</v>
-      </c>
-      <c r="H46" s="6" t="str">
-        <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
-        <v>80.0 min</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H46" s="2" t="str">
+        <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
+        <v>24,000.0 sec</v>
+      </c>
+      <c r="I46" s="2" t="str">
+        <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
+        <v>400.0 min</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>83</v>
       </c>
@@ -2818,30 +3020,33 @@
         <v>77</v>
       </c>
       <c r="C47" t="s">
+        <v>87</v>
+      </c>
+      <c r="D47" t="s">
         <v>78</v>
       </c>
-      <c r="D47">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="E47" s="5">
-        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
-        <v>17000</v>
-      </c>
-      <c r="F47" s="6" t="str">
+      <c r="E47">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="F47">
+        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
+        <v>85000</v>
+      </c>
+      <c r="G47" s="2" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>13.6 sec</v>
       </c>
-      <c r="G47" s="6" t="str">
-        <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
-        <v>1,360.0 sec</v>
-      </c>
-      <c r="H47" s="6" t="str">
-        <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
-        <v>22.7 min</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H47" s="2" t="str">
+        <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
+        <v>6,800.0 sec</v>
+      </c>
+      <c r="I47" s="2" t="str">
+        <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
+        <v>113.3 min</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>84</v>
       </c>
@@ -2849,32 +3054,35 @@
         <v>85</v>
       </c>
       <c r="C48" t="s">
+        <v>89</v>
+      </c>
+      <c r="D48" t="s">
         <v>81</v>
       </c>
-      <c r="D48">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="E48" s="5">
-        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
-        <v>60000</v>
-      </c>
-      <c r="F48" s="6" t="str">
+      <c r="E48">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="F48">
+        <f>VALUE(Table53[[#This Row],[JOB_TIME_old]])*Table53[[#This Row],[Rate]]</f>
+        <v>300000</v>
+      </c>
+      <c r="G48" s="2" t="str">
         <f>TEXT(VALUE(Table53[[#This Row],[JOB_TIME_old]])/15*1.2,"#,##0.0")&amp; " sec"</f>
         <v>48.0 sec</v>
       </c>
-      <c r="G48" s="6" t="str">
-        <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
-        <v>4,800.0 sec</v>
-      </c>
-      <c r="H48" s="6" t="str">
-        <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
-        <v>80.0 min</v>
+      <c r="H48" s="2" t="str">
+        <f>TEXT(Table53[[#This Row],[JOB_TIME]]/15*1.2,"#,##0.0")&amp; " sec"</f>
+        <v>24,000.0 sec</v>
+      </c>
+      <c r="I48" s="2" t="str">
+        <f>TEXT(SUBSTITUTE(Table53[[#This Row],[New Time]]," sec","")/60,"#,##0.0")&amp;" min"</f>
+        <v>400.0 min</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A48">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>